<commit_message>
1. add one result and change the name of ff and fb.
</commit_message>
<xml_diff>
--- a/results/summary_results.xlsx
+++ b/results/summary_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -872,78 +872,74 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
+      <c r="A16" t="inlineStr"/>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Valve</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>adam</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="F16" t="n">
+        <v>256</v>
+      </c>
+      <c r="G16" t="n">
+        <v>200</v>
+      </c>
+      <c r="H16" t="n">
+        <v>92.875</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
         <is>
           <t>lif</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B17" t="inlineStr">
         <is>
           <t>Network</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="C17" t="inlineStr">
         <is>
           <t>Task</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="D17" t="inlineStr">
         <is>
           <t>Optimizer</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="E17" t="inlineStr">
         <is>
           <t>Learning Rate</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="F17" t="inlineStr">
         <is>
           <t>Batch Size</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
+      <c r="G17" t="inlineStr">
         <is>
           <t>Epochs</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr"/>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr"/>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>ff</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Valve</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>adam</t>
-        </is>
-      </c>
-      <c r="E17" t="n">
-        <v>0.0005</v>
-      </c>
-      <c r="F17" t="n">
-        <v>256</v>
-      </c>
-      <c r="G17" t="n">
-        <v>200</v>
-      </c>
-      <c r="H17" t="n">
-        <v>38.5</v>
-      </c>
+      <c r="H17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr"/>
       <c r="B18" t="inlineStr">
         <is>
-          <t>alexnet</t>
+          <t>ff</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -966,180 +962,172 @@
         <v>200</v>
       </c>
       <c r="H18" t="n">
-        <v>43.4375</v>
+        <v>38.5</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr"/>
       <c r="B19" t="inlineStr">
         <is>
+          <t>alexnet</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Valve</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>adam</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="F19" t="n">
+        <v>256</v>
+      </c>
+      <c r="G19" t="n">
+        <v>200</v>
+      </c>
+      <c r="H19" t="n">
+        <v>43.4375</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr"/>
+      <c r="B20" t="inlineStr">
+        <is>
           <t>resnet</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Valve</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>adam</t>
-        </is>
-      </c>
-      <c r="E19" t="n">
-        <v>0.0005</v>
-      </c>
-      <c r="F19" t="n">
-        <v>256</v>
-      </c>
-      <c r="G19" t="n">
-        <v>200</v>
-      </c>
-      <c r="H19" t="n">
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Valve</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>adam</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="F20" t="n">
+        <v>256</v>
+      </c>
+      <c r="G20" t="n">
+        <v>200</v>
+      </c>
+      <c r="H20" t="n">
         <v>33.375</v>
       </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>alif</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Network</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Task</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>Optimizer</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>Learning Rate</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>Batch Size</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>Epochs</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr"/>
       <c r="B21" t="inlineStr">
         <is>
+          <t>fb</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Valve</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>adam</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="F21" t="n">
+        <v>256</v>
+      </c>
+      <c r="G21" t="n">
+        <v>200</v>
+      </c>
+      <c r="H21" t="n">
+        <v>88.5</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>alif</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Network</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Optimizer</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Learning Rate</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Batch Size</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Epochs</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr"/>
+      <c r="B23" t="inlineStr">
+        <is>
           <t>ff</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Valve</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>adam</t>
-        </is>
-      </c>
-      <c r="E21" t="n">
-        <v>0.0005</v>
-      </c>
-      <c r="F21" t="n">
-        <v>256</v>
-      </c>
-      <c r="G21" t="n">
-        <v>200</v>
-      </c>
-      <c r="H21" t="n">
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Valve</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>adam</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="F23" t="n">
+        <v>256</v>
+      </c>
+      <c r="G23" t="n">
+        <v>200</v>
+      </c>
+      <c r="H23" t="n">
         <v>40.625</v>
       </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr"/>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>alexnet</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>Valve</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>adam</t>
-        </is>
-      </c>
-      <c r="E22" t="n">
-        <v>0.0005</v>
-      </c>
-      <c r="F22" t="n">
-        <v>256</v>
-      </c>
-      <c r="G22" t="n">
-        <v>200</v>
-      </c>
-      <c r="H22" t="n">
-        <v>39.5</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>plif</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Network</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>Task</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>Optimizer</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>Learning Rate</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>Batch Size</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>Epochs</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr"/>
       <c r="B24" t="inlineStr">
         <is>
-          <t>ff</t>
+          <t>alexnet</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1162,66 +1150,164 @@
         <v>200</v>
       </c>
       <c r="H24" t="n">
-        <v>40.4375</v>
+        <v>39.5</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr"/>
       <c r="B25" t="inlineStr">
         <is>
+          <t>fb</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Valve</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>adam</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="F25" t="n">
+        <v>256</v>
+      </c>
+      <c r="G25" t="n">
+        <v>200</v>
+      </c>
+      <c r="H25" t="n">
+        <v>22.9375</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>plif</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Network</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Optimizer</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Learning Rate</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Batch Size</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Epochs</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr"/>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>ff</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Valve</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>adam</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="F27" t="n">
+        <v>256</v>
+      </c>
+      <c r="G27" t="n">
+        <v>200</v>
+      </c>
+      <c r="H27" t="n">
+        <v>40.4375</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr"/>
+      <c r="B28" t="inlineStr">
+        <is>
           <t>alexnet</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>Valve</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>adam</t>
-        </is>
-      </c>
-      <c r="E25" t="n">
-        <v>0.0005</v>
-      </c>
-      <c r="F25" t="n">
-        <v>256</v>
-      </c>
-      <c r="G25" t="n">
-        <v>200</v>
-      </c>
-      <c r="H25" t="n">
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Valve</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>adam</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="F28" t="n">
+        <v>256</v>
+      </c>
+      <c r="G28" t="n">
+        <v>200</v>
+      </c>
+      <c r="H28" t="n">
         <v>44.375</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" t="inlineStr"/>
-      <c r="B26" t="inlineStr">
+    <row r="29">
+      <c r="A29" t="inlineStr"/>
+      <c r="B29" t="inlineStr">
         <is>
           <t>resnet</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>Valve</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>adam</t>
-        </is>
-      </c>
-      <c r="E26" t="n">
-        <v>0.0005</v>
-      </c>
-      <c r="F26" t="n">
-        <v>256</v>
-      </c>
-      <c r="G26" t="n">
-        <v>200</v>
-      </c>
-      <c r="H26" t="n">
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Valve</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>adam</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="F29" t="n">
+        <v>256</v>
+      </c>
+      <c r="G29" t="n">
+        <v>200</v>
+      </c>
+      <c r="H29" t="n">
         <v>34.0625</v>
       </c>
     </row>

</xml_diff>

<commit_message>
1. add one result.
</commit_message>
<xml_diff>
--- a/results/summary_results.xlsx
+++ b/results/summary_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -898,50 +898,34 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>lif</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Network</t>
-        </is>
-      </c>
+      <c r="A17" t="inlineStr"/>
+      <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Task</t>
+          <t>Valve</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Optimizer</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>Learning Rate</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>Batch Size</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>Epochs</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr"/>
+          <t>adam</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="F17" t="n">
+        <v>256</v>
+      </c>
+      <c r="G17" t="n">
+        <v>200</v>
+      </c>
+      <c r="H17" t="n">
+        <v>93.375</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr"/>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>ff</t>
-        </is>
-      </c>
+      <c r="B18" t="inlineStr"/>
       <c r="C18" t="inlineStr">
         <is>
           <t>Valve</t>
@@ -962,44 +946,52 @@
         <v>200</v>
       </c>
       <c r="H18" t="n">
-        <v>38.5</v>
+        <v>92.875</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr"/>
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>lif</t>
+        </is>
+      </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>alexnet</t>
+          <t>Network</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Valve</t>
+          <t>Task</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>adam</t>
-        </is>
-      </c>
-      <c r="E19" t="n">
-        <v>0.0005</v>
-      </c>
-      <c r="F19" t="n">
-        <v>256</v>
-      </c>
-      <c r="G19" t="n">
-        <v>200</v>
-      </c>
-      <c r="H19" t="n">
-        <v>43.4375</v>
-      </c>
+          <t>Optimizer</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Learning Rate</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Batch Size</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Epochs</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr"/>
       <c r="B20" t="inlineStr">
         <is>
-          <t>resnet</t>
+          <t>ff</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1022,14 +1014,14 @@
         <v>200</v>
       </c>
       <c r="H20" t="n">
-        <v>33.375</v>
+        <v>38.5</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr"/>
       <c r="B21" t="inlineStr">
         <is>
-          <t>fb</t>
+          <t>alexnet</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1052,52 +1044,44 @@
         <v>200</v>
       </c>
       <c r="H21" t="n">
-        <v>88.5</v>
+        <v>43.4375</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>alif</t>
-        </is>
-      </c>
+      <c r="A22" t="inlineStr"/>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Network</t>
+          <t>resnet</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Task</t>
+          <t>Valve</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Optimizer</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>Learning Rate</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>Batch Size</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>Epochs</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr"/>
+          <t>adam</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="F22" t="n">
+        <v>256</v>
+      </c>
+      <c r="G22" t="n">
+        <v>200</v>
+      </c>
+      <c r="H22" t="n">
+        <v>33.375</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr"/>
       <c r="B23" t="inlineStr">
         <is>
-          <t>ff</t>
+          <t>fb</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1120,44 +1104,52 @@
         <v>200</v>
       </c>
       <c r="H23" t="n">
-        <v>40.625</v>
+        <v>88.5</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr"/>
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>alif</t>
+        </is>
+      </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>alexnet</t>
+          <t>Network</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Valve</t>
+          <t>Task</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>adam</t>
-        </is>
-      </c>
-      <c r="E24" t="n">
-        <v>0.0005</v>
-      </c>
-      <c r="F24" t="n">
-        <v>256</v>
-      </c>
-      <c r="G24" t="n">
-        <v>200</v>
-      </c>
-      <c r="H24" t="n">
-        <v>39.5</v>
-      </c>
+          <t>Optimizer</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Learning Rate</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Batch Size</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Epochs</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr"/>
       <c r="B25" t="inlineStr">
         <is>
-          <t>fb</t>
+          <t>ff</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1180,52 +1172,44 @@
         <v>200</v>
       </c>
       <c r="H25" t="n">
-        <v>22.9375</v>
+        <v>40.625</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>plif</t>
-        </is>
-      </c>
+      <c r="A26" t="inlineStr"/>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Network</t>
+          <t>alexnet</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Task</t>
+          <t>Valve</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Optimizer</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>Learning Rate</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>Batch Size</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>Epochs</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr"/>
+          <t>adam</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="F26" t="n">
+        <v>256</v>
+      </c>
+      <c r="G26" t="n">
+        <v>200</v>
+      </c>
+      <c r="H26" t="n">
+        <v>39.5</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr"/>
       <c r="B27" t="inlineStr">
         <is>
-          <t>ff</t>
+          <t>fb</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1248,66 +1232,134 @@
         <v>200</v>
       </c>
       <c r="H27" t="n">
-        <v>40.4375</v>
+        <v>22.9375</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr"/>
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>plif</t>
+        </is>
+      </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>alexnet</t>
+          <t>Network</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Valve</t>
+          <t>Task</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>adam</t>
-        </is>
-      </c>
-      <c r="E28" t="n">
-        <v>0.0005</v>
-      </c>
-      <c r="F28" t="n">
-        <v>256</v>
-      </c>
-      <c r="G28" t="n">
-        <v>200</v>
-      </c>
-      <c r="H28" t="n">
-        <v>44.375</v>
-      </c>
+          <t>Optimizer</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Learning Rate</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Batch Size</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Epochs</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr"/>
       <c r="B29" t="inlineStr">
         <is>
+          <t>ff</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Valve</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>adam</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="F29" t="n">
+        <v>256</v>
+      </c>
+      <c r="G29" t="n">
+        <v>200</v>
+      </c>
+      <c r="H29" t="n">
+        <v>40.4375</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr"/>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>alexnet</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Valve</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>adam</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="F30" t="n">
+        <v>256</v>
+      </c>
+      <c r="G30" t="n">
+        <v>200</v>
+      </c>
+      <c r="H30" t="n">
+        <v>44.375</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr"/>
+      <c r="B31" t="inlineStr">
+        <is>
           <t>resnet</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>Valve</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>adam</t>
-        </is>
-      </c>
-      <c r="E29" t="n">
-        <v>0.0005</v>
-      </c>
-      <c r="F29" t="n">
-        <v>256</v>
-      </c>
-      <c r="G29" t="n">
-        <v>200</v>
-      </c>
-      <c r="H29" t="n">
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Valve</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>adam</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="F31" t="n">
+        <v>256</v>
+      </c>
+      <c r="G31" t="n">
+        <v>200</v>
+      </c>
+      <c r="H31" t="n">
         <v>34.0625</v>
       </c>
     </row>

</xml_diff>

<commit_message>
1.Add some results and processing codes.
</commit_message>
<xml_diff>
--- a/results/summary_results.xlsx
+++ b/results/summary_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -920,7 +920,7 @@
         <v>200</v>
       </c>
       <c r="H17" t="n">
-        <v>93.375</v>
+        <v>92.875</v>
       </c>
     </row>
     <row r="18">
@@ -943,57 +943,41 @@
         <v>256</v>
       </c>
       <c r="G18" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="H18" t="n">
-        <v>92.875</v>
+        <v>93.875</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>lif</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Network</t>
-        </is>
-      </c>
+      <c r="A19" t="inlineStr"/>
+      <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Task</t>
+          <t>Valve</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Optimizer</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>Learning Rate</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>Batch Size</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>Epochs</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr"/>
+          <t>adam</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="F19" t="n">
+        <v>256</v>
+      </c>
+      <c r="G19" t="n">
+        <v>100</v>
+      </c>
+      <c r="H19" t="n">
+        <v>93.9375</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr"/>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>ff</t>
-        </is>
-      </c>
+      <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr">
         <is>
           <t>Valve</t>
@@ -1011,19 +995,15 @@
         <v>256</v>
       </c>
       <c r="G20" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="H20" t="n">
-        <v>38.5</v>
+        <v>93.3125</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr"/>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>alexnet</t>
-        </is>
-      </c>
+      <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr">
         <is>
           <t>Valve</t>
@@ -1041,19 +1021,15 @@
         <v>256</v>
       </c>
       <c r="G21" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="H21" t="n">
-        <v>43.4375</v>
+        <v>94.3125</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr"/>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>resnet</t>
-        </is>
-      </c>
+      <c r="B22" t="inlineStr"/>
       <c r="C22" t="inlineStr">
         <is>
           <t>Valve</t>
@@ -1071,85 +1047,85 @@
         <v>256</v>
       </c>
       <c r="G22" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="H22" t="n">
-        <v>33.375</v>
+        <v>92.375</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr"/>
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>lif</t>
+        </is>
+      </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>fb</t>
+          <t>Network</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Valve</t>
+          <t>Task</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>adam</t>
-        </is>
-      </c>
-      <c r="E23" t="n">
-        <v>0.0005</v>
-      </c>
-      <c r="F23" t="n">
-        <v>256</v>
-      </c>
-      <c r="G23" t="n">
-        <v>200</v>
-      </c>
-      <c r="H23" t="n">
-        <v>88.5</v>
-      </c>
+          <t>Optimizer</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Learning Rate</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Batch Size</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Epochs</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr"/>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>alif</t>
-        </is>
-      </c>
+      <c r="A24" t="inlineStr"/>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Network</t>
+          <t>ff</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Task</t>
+          <t>Valve</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Optimizer</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>Learning Rate</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>Batch Size</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>Epochs</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr"/>
+          <t>adam</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="F24" t="n">
+        <v>256</v>
+      </c>
+      <c r="G24" t="n">
+        <v>200</v>
+      </c>
+      <c r="H24" t="n">
+        <v>38.5</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr"/>
       <c r="B25" t="inlineStr">
         <is>
-          <t>ff</t>
+          <t>alexnet</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1172,14 +1148,14 @@
         <v>200</v>
       </c>
       <c r="H25" t="n">
-        <v>40.625</v>
+        <v>43.4375</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr"/>
       <c r="B26" t="inlineStr">
         <is>
-          <t>alexnet</t>
+          <t>resnet</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1202,7 +1178,7 @@
         <v>200</v>
       </c>
       <c r="H26" t="n">
-        <v>39.5</v>
+        <v>33.375</v>
       </c>
     </row>
     <row r="27">
@@ -1232,13 +1208,13 @@
         <v>200</v>
       </c>
       <c r="H27" t="n">
-        <v>22.9375</v>
+        <v>88.5</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>plif</t>
+          <t>alif</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1300,7 +1276,7 @@
         <v>200</v>
       </c>
       <c r="H29" t="n">
-        <v>40.4375</v>
+        <v>40.625</v>
       </c>
     </row>
     <row r="30">
@@ -1330,36 +1306,164 @@
         <v>200</v>
       </c>
       <c r="H30" t="n">
-        <v>44.375</v>
+        <v>39.5</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr"/>
       <c r="B31" t="inlineStr">
         <is>
+          <t>fb</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Valve</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>adam</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="F31" t="n">
+        <v>256</v>
+      </c>
+      <c r="G31" t="n">
+        <v>200</v>
+      </c>
+      <c r="H31" t="n">
+        <v>22.9375</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>plif</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Network</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Optimizer</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Learning Rate</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Batch Size</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Epochs</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr"/>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>ff</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Valve</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>adam</t>
+        </is>
+      </c>
+      <c r="E33" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="F33" t="n">
+        <v>256</v>
+      </c>
+      <c r="G33" t="n">
+        <v>200</v>
+      </c>
+      <c r="H33" t="n">
+        <v>40.4375</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr"/>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>alexnet</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Valve</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>adam</t>
+        </is>
+      </c>
+      <c r="E34" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="F34" t="n">
+        <v>256</v>
+      </c>
+      <c r="G34" t="n">
+        <v>200</v>
+      </c>
+      <c r="H34" t="n">
+        <v>44.375</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr"/>
+      <c r="B35" t="inlineStr">
+        <is>
           <t>resnet</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>Valve</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>adam</t>
-        </is>
-      </c>
-      <c r="E31" t="n">
-        <v>0.0005</v>
-      </c>
-      <c r="F31" t="n">
-        <v>256</v>
-      </c>
-      <c r="G31" t="n">
-        <v>200</v>
-      </c>
-      <c r="H31" t="n">
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Valve</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>adam</t>
+        </is>
+      </c>
+      <c r="E35" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="F35" t="n">
+        <v>256</v>
+      </c>
+      <c r="G35" t="n">
+        <v>200</v>
+      </c>
+      <c r="H35" t="n">
         <v>34.0625</v>
       </c>
     </row>

</xml_diff>